<commit_message>
Added a popup for when Excel tables are created
</commit_message>
<xml_diff>
--- a/aprovados.xlsx
+++ b/aprovados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,17 +452,47 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Marcelo</t>
+          <t>Jenivaldo</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Marcelo</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Marcos</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Matias</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the entry fucntions to use .strip
</commit_message>
<xml_diff>
--- a/aprovados.xlsx
+++ b/aprovados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jenivaldo</t>
+          <t>Genivaldo</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -468,7 +468,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Marcelo</t>
+          <t>José</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -478,20 +478,30 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>João</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Marcelo</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Matias</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B7" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>